<commit_message>
add some bugs in the BugReport.xlsx and cleaned up the test templates
</commit_message>
<xml_diff>
--- a/Testing/Test Procedures/BugReport.xlsx
+++ b/Testing/Test Procedures/BugReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Bug ID</t>
   </si>
@@ -44,6 +44,63 @@
   </si>
   <si>
     <t>Reported On</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>error page on po creation</t>
+  </si>
+  <si>
+    <t>purchaseordercontroler.cs</t>
+  </si>
+  <si>
+    <t>create po and submit it then try to create a second one</t>
+  </si>
+  <si>
+    <t>unfixed</t>
+  </si>
+  <si>
+    <t>Mathew</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>no validation on po creation</t>
+  </si>
+  <si>
+    <t>create po with none valid input</t>
+  </si>
+  <si>
+    <t>page for /RECEIVING_LOG/findPO/orig not found when looking up a rl</t>
+  </si>
+  <si>
+    <t>receivinglogcontroler.cs</t>
+  </si>
+  <si>
+    <t>look up any record in receiving log</t>
+  </si>
+  <si>
+    <t>no validation on begin receiving log</t>
+  </si>
+  <si>
+    <t>look up any record with incorrect information</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>deletes invalid input in the MSRP field and states it is required</t>
+  </si>
+  <si>
+    <t>itemmanagementcontroler.cs</t>
+  </si>
+  <si>
+    <t>input 'something' into MSRP on item creation</t>
+  </si>
+  <si>
+    <t>Nate</t>
   </si>
 </sst>
 </file>
@@ -79,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,16 +419,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
@@ -408,6 +466,136 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1">
+        <v>41691</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1">
+        <v>41691</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1">
+        <v>41691</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="1">
+        <v>41691</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1">
+        <v>41687</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>